<commit_message>
Add `task-6` in `game-theory`
</commit_message>
<xml_diff>
--- a/3-course-6-semester/game-theory/КТ1/Бронников ПМ-1901 - Задача 1.xlsx
+++ b/3-course-6-semester/game-theory/КТ1/Бронников ПМ-1901 - Задача 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bronn\Documents\github\university\3-course-6-semester\game-theory\КТ1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AD709C-81BF-41BC-A10C-6D4CE4FC0E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353D3CAE-8529-4F79-89DA-B6ED3F359E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C475A2DF-953A-4926-B4CF-8AED05C01FF6}"/>
   </bookViews>
@@ -4064,8 +4064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5909A454-3C39-4F6B-9B44-98C203526564}">
   <dimension ref="A1:DA122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5013,7 +5013,7 @@
         <v>-1.95</v>
       </c>
       <c r="C20" s="19">
-        <f t="shared" ref="C20:R51" si="4">$A20*C$17+C$17</f>
+        <f t="shared" ref="C20:R42" si="4">$A20*C$17+C$17</f>
         <v>0.95</v>
       </c>
       <c r="D20" s="15">
@@ -6097,7 +6097,7 @@
         <v>-2.3630000000000018</v>
       </c>
       <c r="BO22" s="15">
-        <f t="shared" ref="D22:BO85" si="7">$A22*BO$17+BO$17</f>
+        <f t="shared" ref="D22:BO26" si="7">$A22*BO$17+BO$17</f>
         <v>-2.4140000000000015</v>
       </c>
       <c r="BP22" s="15">
@@ -7749,7 +7749,7 @@
         <v>-1.7680000000000007</v>
       </c>
       <c r="BN26" s="15">
-        <f t="shared" ref="BN26:CC89" si="8">$A26*BN$17+BN$17</f>
+        <f t="shared" ref="BN26:CC51" si="8">$A26*BN$17+BN$17</f>
         <v>-1.8070000000000008</v>
       </c>
       <c r="BO26" s="15">
@@ -7769,7 +7769,7 @@
         <v>-1.9630000000000005</v>
       </c>
       <c r="BS26" s="15">
-        <f t="shared" ref="BS26:CH89" si="9">$A26*BS$17+BS$17</f>
+        <f t="shared" ref="BS26:CH26" si="9">$A26*BS$17+BS$17</f>
         <v>-2.0020000000000007</v>
       </c>
       <c r="BT26" s="15">
@@ -7833,7 +7833,7 @@
         <v>-2.5870000000000011</v>
       </c>
       <c r="CI26" s="15">
-        <f t="shared" ref="CI26:CX89" si="10">$A26*CI$17+CI$17</f>
+        <f t="shared" ref="CI26:CX26" si="10">$A26*CI$17+CI$17</f>
         <v>-2.6260000000000012</v>
       </c>
       <c r="CJ26" s="15">
@@ -7897,7 +7897,7 @@
         <v>-3.2109999999999967</v>
       </c>
       <c r="CY26" s="20">
-        <f t="shared" ref="BP26:CY89" si="11">$A26*CY$17+CY$17</f>
+        <f t="shared" ref="BP26:CY34" si="11">$A26*CY$17+CY$17</f>
         <v>-3.2499999999999973</v>
       </c>
       <c r="DA26" s="25">
@@ -7975,7 +7975,7 @@
         <v>5.999999999999972E-2</v>
       </c>
       <c r="S27" s="15">
-        <f t="shared" ref="S27:AH90" si="12">$A27*S$17+S$17</f>
+        <f t="shared" ref="S27:AH43" si="12">$A27*S$17+S$17</f>
         <v>2.3999999999999744E-2</v>
       </c>
       <c r="T27" s="15">
@@ -8039,7 +8039,7 @@
         <v>-0.51600000000000024</v>
       </c>
       <c r="AI27" s="15">
-        <f t="shared" ref="AI27:AX90" si="13">$A27*AI$17+AI$17</f>
+        <f t="shared" ref="AI27:AX42" si="13">$A27*AI$17+AI$17</f>
         <v>-0.55200000000000027</v>
       </c>
       <c r="AJ27" s="15">
@@ -8103,7 +8103,7 @@
         <v>-1.0920000000000005</v>
       </c>
       <c r="AY27" s="15">
-        <f t="shared" ref="AY27:BN90" si="14">$A27*AY$17+AY$17</f>
+        <f t="shared" ref="AY27:BN56" si="14">$A27*AY$17+AY$17</f>
         <v>-1.1280000000000001</v>
       </c>
       <c r="AZ27" s="15">
@@ -11077,7 +11077,7 @@
         <v>-0.73999999999999888</v>
       </c>
       <c r="BR34" s="15">
-        <f t="shared" ref="BR34:CG97" si="15">$A34*BR$17+BR$17</f>
+        <f t="shared" ref="BR34:CG50" si="15">$A34*BR$17+BR$17</f>
         <v>-0.75499999999999856</v>
       </c>
       <c r="BS34" s="15">
@@ -11141,7 +11141,7 @@
         <v>-0.97999999999999865</v>
       </c>
       <c r="CH34" s="15">
-        <f t="shared" ref="CH34:CW97" si="16">$A34*CH$17+CH$17</f>
+        <f t="shared" ref="CH34:CW49" si="16">$A34*CH$17+CH$17</f>
         <v>-0.99499999999999789</v>
       </c>
       <c r="CI34" s="15">
@@ -11205,7 +11205,7 @@
         <v>-1.2199999999999962</v>
       </c>
       <c r="CX34" s="15">
-        <f t="shared" ref="CX34:CY97" si="17">$A34*CX$17+CX$17</f>
+        <f t="shared" ref="CX34:CY48" si="17">$A34*CX$17+CX$17</f>
         <v>-1.2349999999999959</v>
       </c>
       <c r="CY34" s="20">
@@ -14153,7 +14153,7 @@
         <v>-8.7000000000000521E-2</v>
       </c>
       <c r="K42" s="15">
-        <f t="shared" ref="K42:Z105" si="18">$A42*K$17+K$17</f>
+        <f t="shared" ref="K42:Z57" si="18">$A42*K$17+K$17</f>
         <v>-7.8000000000000458E-2</v>
       </c>
       <c r="L42" s="15">
@@ -14309,7 +14309,7 @@
         <v>0.26400000000000201</v>
       </c>
       <c r="AX42" s="15">
-        <f t="shared" ref="AX42:BM105" si="19">$A42*AX$17+AX$17</f>
+        <f t="shared" ref="AX42:BM57" si="19">$A42*AX$17+AX$17</f>
         <v>0.27300000000000213</v>
       </c>
       <c r="AY42" s="15">
@@ -14535,7 +14535,7 @@
         <v>-0.79999999999999893</v>
       </c>
       <c r="C43" s="19">
-        <f t="shared" ref="C43:R74" si="20">$A43*C$17+C$17</f>
+        <f t="shared" ref="C43:R58" si="20">$A43*C$17+C$17</f>
         <v>-0.20000000000000107</v>
       </c>
       <c r="D43" s="15">
@@ -14659,7 +14659,7 @@
         <v>0.16000000000000103</v>
       </c>
       <c r="AH43" s="15">
-        <f t="shared" ref="AH43:AW106" si="21">$A43*AH$17+AH$17</f>
+        <f t="shared" ref="AH43:AW60" si="21">$A43*AH$17+AH$17</f>
         <v>0.17200000000000104</v>
       </c>
       <c r="AI43" s="15">
@@ -15045,7 +15045,7 @@
         <v>9.5000000000000528E-2</v>
       </c>
       <c r="AA44" s="15">
-        <f t="shared" ref="AA44:AP107" si="22">$A44*AA$17+AA$17</f>
+        <f t="shared" ref="AA44:AP61" si="22">$A44*AA$17+AA$17</f>
         <v>0.1100000000000006</v>
       </c>
       <c r="AB44" s="15">
@@ -17411,7 +17411,7 @@
         <v>2.4100000000000055</v>
       </c>
       <c r="CW49" s="15">
-        <f t="shared" ref="CW49:CY112" si="23">$A49*CW$17+CW$17</f>
+        <f t="shared" ref="CW49:CY67" si="23">$A49*CW$17+CW$17</f>
         <v>2.4400000000000053</v>
       </c>
       <c r="CX49" s="15">
@@ -17765,7 +17765,7 @@
         <v>2.1560000000000068</v>
       </c>
       <c r="CH50" s="15">
-        <f t="shared" ref="CH50:CW113" si="24">$A50*CH$17+CH$17</f>
+        <f t="shared" ref="CH50:CW68" si="24">$A50*CH$17+CH$17</f>
         <v>2.1890000000000072</v>
       </c>
       <c r="CI50" s="15">
@@ -18123,7 +18123,7 @@
         <v>1.8480000000000054</v>
       </c>
       <c r="BT51" s="15">
-        <f t="shared" ref="BT51:CI114" si="25">$A51*BT$17+BT$17</f>
+        <f t="shared" ref="BT51:CI67" si="25">$A51*BT$17+BT$17</f>
         <v>1.8840000000000057</v>
       </c>
       <c r="BU51" s="15">
@@ -18517,7 +18517,7 @@
         <v>1.807000000000005</v>
       </c>
       <c r="BO52" s="15">
-        <f t="shared" ref="BO52:CD115" si="26">$A52*BO$17+BO$17</f>
+        <f t="shared" ref="BO52:CD68" si="26">$A52*BO$17+BO$17</f>
         <v>1.8460000000000052</v>
       </c>
       <c r="BP52" s="15">
@@ -20579,7 +20579,7 @@
         <v>2.3940000000000055</v>
       </c>
       <c r="BM57" s="15">
-        <f t="shared" ref="BM57:CB119" si="27">$A57*BM$17+BM$17</f>
+        <f t="shared" ref="BM57:CB84" si="27">$A57*BM$17+BM$17</f>
         <v>2.4480000000000053</v>
       </c>
       <c r="BN57" s="15">
@@ -20805,7 +20805,7 @@
         <v>-0.1519999999999998</v>
       </c>
       <c r="R58" s="15">
-        <f t="shared" ref="R58:AG119" si="28">$A58*R$17+R$17</f>
+        <f t="shared" ref="R58:AG73" si="28">$A58*R$17+R$17</f>
         <v>-9.4999999999999724E-2</v>
       </c>
       <c r="S58" s="15">
@@ -20933,7 +20933,7 @@
         <v>1.6720000000000037</v>
       </c>
       <c r="AX58" s="15">
-        <f t="shared" ref="AX58:BM119" si="29">$A58*AX$17+AX$17</f>
+        <f t="shared" ref="AX58:BM91" si="29">$A58*AX$17+AX$17</f>
         <v>1.7290000000000036</v>
       </c>
       <c r="AY58" s="15">
@@ -21159,7 +21159,7 @@
         <v>1.2073675392798577E-15</v>
       </c>
       <c r="C59" s="19">
-        <f t="shared" ref="C59:R90" si="30">$A59*C$17+C$17</f>
+        <f t="shared" ref="C59:R74" si="30">$A59*C$17+C$17</f>
         <v>-1.0000000000000011</v>
       </c>
       <c r="D59" s="15">
@@ -22127,7 +22127,7 @@
         <v>1.1440000000000023</v>
       </c>
       <c r="AL61" s="15">
-        <f t="shared" ref="AL61:BA119" si="31">$A61*AL$17+AL$17</f>
+        <f t="shared" ref="AL61:BA76" si="31">$A61*AL$17+AL$17</f>
         <v>1.2100000000000024</v>
       </c>
       <c r="AM61" s="15">
@@ -22525,7 +22525,7 @@
         <v>0.92000000000000182</v>
       </c>
       <c r="AH62" s="15">
-        <f t="shared" ref="AH62:AW119" si="32">$A62*AH$17+AH$17</f>
+        <f t="shared" ref="AH62:AW77" si="32">$A62*AH$17+AH$17</f>
         <v>0.98900000000000188</v>
       </c>
       <c r="AI62" s="15">
@@ -25185,7 +25185,7 @@
         <v>4.9880000000000084</v>
       </c>
       <c r="BZ68" s="15">
-        <f t="shared" ref="BZ68:CO119" si="33">$A68*BZ$17+BZ$17</f>
+        <f t="shared" ref="BZ68:CO90" si="33">$A68*BZ$17+BZ$17</f>
         <v>5.0750000000000082</v>
       </c>
       <c r="CA68" s="15">
@@ -25253,7 +25253,7 @@
         <v>6.4670000000000059</v>
       </c>
       <c r="CQ68" s="15">
-        <f t="shared" ref="CQ68:CY119" si="34">$A68*CQ$17+CQ$17</f>
+        <f t="shared" ref="CQ68:CY68" si="34">$A68*CQ$17+CQ$17</f>
         <v>6.5540000000000056</v>
       </c>
       <c r="CR68" s="15">
@@ -25663,7 +25663,7 @@
         <v>6.6000000000000068</v>
       </c>
       <c r="CP69" s="15">
-        <f t="shared" ref="CP69:CY119" si="35">$A69*CP$17+CP$17</f>
+        <f t="shared" ref="CP69:CY89" si="35">$A69*CP$17+CP$17</f>
         <v>6.6900000000000066</v>
       </c>
       <c r="CQ69" s="15">
@@ -27429,7 +27429,7 @@
         <v>-0.27999999999999953</v>
       </c>
       <c r="R74" s="15">
-        <f t="shared" ref="R74:AG119" si="36">$A74*R$17+R$17</f>
+        <f t="shared" ref="R74:AG89" si="36">$A74*R$17+R$17</f>
         <v>-0.17499999999999943</v>
       </c>
       <c r="S74" s="15">
@@ -27783,7 +27783,7 @@
         <v>0.80000000000000149</v>
       </c>
       <c r="C75" s="19">
-        <f t="shared" ref="C75:R119" si="37">$A75*C$17+C$17</f>
+        <f t="shared" ref="C75:R90" si="37">$A75*C$17+C$17</f>
         <v>-1.8000000000000016</v>
       </c>
       <c r="D75" s="15">
@@ -28795,7 +28795,7 @@
         <v>3.2300000000000058</v>
       </c>
       <c r="AW77" s="15">
-        <f t="shared" ref="AW77:BL119" si="38">$A77*AW$17+AW$17</f>
+        <f t="shared" ref="AW77:BL92" si="38">$A77*AW$17+AW$17</f>
         <v>3.3440000000000056</v>
       </c>
       <c r="AX77" s="15">
@@ -29149,7 +29149,7 @@
         <v>1.5600000000000027</v>
       </c>
       <c r="AH78" s="15">
-        <f t="shared" ref="AH78:AW119" si="39">$A78*AH$17+AH$17</f>
+        <f t="shared" ref="AH78:AW93" si="39">$A78*AH$17+AH$17</f>
         <v>1.6770000000000029</v>
       </c>
       <c r="AI78" s="15">
@@ -31781,7 +31781,7 @@
         <v>6.7950000000000115</v>
       </c>
       <c r="BS84" s="15">
-        <f t="shared" ref="BS84:CH119" si="40">$A84*BS$17+BS$17</f>
+        <f t="shared" ref="BS84:CH101" si="40">$A84*BS$17+BS$17</f>
         <v>6.9300000000000122</v>
       </c>
       <c r="BT84" s="15">
@@ -32175,7 +32175,7 @@
         <v>6.2560000000000109</v>
       </c>
       <c r="BN85" s="15">
-        <f t="shared" ref="BN85:CC119" si="43">$A85*BN$17+BN$17</f>
+        <f t="shared" ref="BN85:CC102" si="43">$A85*BN$17+BN$17</f>
         <v>6.3940000000000108</v>
       </c>
       <c r="BO85" s="15">
@@ -34053,7 +34053,7 @@
         <v>-0.40799999999999925</v>
       </c>
       <c r="R90" s="15">
-        <f t="shared" ref="R90:AG119" si="44">$A90*R$17+R$17</f>
+        <f t="shared" ref="R90:AG105" si="44">$A90*R$17+R$17</f>
         <v>-0.25499999999999912</v>
       </c>
       <c r="S90" s="15">
@@ -34337,7 +34337,7 @@
         <v>10.455000000000016</v>
       </c>
       <c r="CK90" s="15">
-        <f t="shared" ref="CK90:CY119" si="45">$A90*CK$17+CK$17</f>
+        <f t="shared" ref="CK90:CY105" si="45">$A90*CK$17+CK$17</f>
         <v>10.608000000000015</v>
       </c>
       <c r="CL90" s="15">
@@ -34407,7 +34407,7 @@
         <v>1.6000000000000021</v>
       </c>
       <c r="C91" s="19">
-        <f t="shared" ref="C91:R119" si="46">$A91*C$17+C$17</f>
+        <f t="shared" ref="C91:R106" si="46">$A91*C$17+C$17</f>
         <v>-2.6000000000000023</v>
       </c>
       <c r="D91" s="15">
@@ -34743,7 +34743,7 @@
         <v>10.348000000000017</v>
       </c>
       <c r="CI91" s="15">
-        <f t="shared" ref="CI91:CX119" si="47">$A91*CI$17+CI$17</f>
+        <f t="shared" ref="CI91:CX106" si="47">$A91*CI$17+CI$17</f>
         <v>10.504000000000017</v>
       </c>
       <c r="CJ91" s="15">
@@ -35069,7 +35069,7 @@
         <v>7.0490000000000119</v>
       </c>
       <c r="BM92" s="15">
-        <f t="shared" ref="BM92:CB119" si="48">$A92*BM$17+BM$17</f>
+        <f t="shared" ref="BM92:CB116" si="48">$A92*BM$17+BM$17</f>
         <v>7.2080000000000126</v>
       </c>
       <c r="BN92" s="15">
@@ -35419,7 +35419,7 @@
         <v>4.5900000000000079</v>
       </c>
       <c r="AW93" s="15">
-        <f t="shared" ref="AW93:BL119" si="49">$A93*AW$17+AW$17</f>
+        <f t="shared" ref="AW93:BL108" si="49">$A93*AW$17+AW$17</f>
         <v>4.7520000000000078</v>
       </c>
       <c r="AX93" s="15">
@@ -35773,7 +35773,7 @@
         <v>2.2000000000000037</v>
       </c>
       <c r="AH94" s="15">
-        <f t="shared" ref="AH94:AW119" si="50">$A94*AH$17+AH$17</f>
+        <f t="shared" ref="AH94:AW109" si="50">$A94*AH$17+AH$17</f>
         <v>2.3650000000000038</v>
       </c>
       <c r="AI94" s="15">
@@ -39233,7 +39233,7 @@
         <v>9.5130000000000141</v>
       </c>
       <c r="BS102" s="15">
-        <f t="shared" ref="BS102:CH119" si="51">$A102*BS$17+BS$17</f>
+        <f t="shared" ref="BS102:CH115" si="51">$A102*BS$17+BS$17</f>
         <v>9.7020000000000142</v>
       </c>
       <c r="BT102" s="15">

</xml_diff>